<commit_message>
Add documentation for DATE, SIN and PV functions
</commit_message>
<xml_diff>
--- a/xlsx/tests/docs/DATE.xlsx
+++ b/xlsx/tests/docs/DATE.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\steve\Documents\IronCalc work\Function descriptions\Date and Time\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\steve\Documents\IronCalc work\IronCalc-clone\IronCalc-SF\xlsx\tests\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{443ECD5D-BBC2-4C12-B0BD-C579F6B3F12F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D590615F-3FC3-4F20-8FA4-D55D11CA56D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Year</t>
   </si>
@@ -49,6 +49,9 @@
   <si>
     <t>Serial Number
 (General Format)</t>
+  </si>
+  <si>
+    <t>Formula Text</t>
   </si>
 </sst>
 </file>
@@ -92,7 +95,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -101,9 +104,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -441,20 +441,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="300" zoomScaleNormal="300" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="10.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.85546875" customWidth="1"/>
-    <col min="5" max="5" width="22.85546875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="21" style="1" customWidth="1"/>
+    <col min="6" max="6" width="24.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -467,11 +468,14 @@
       <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1905</v>
       </c>
@@ -485,12 +489,16 @@
         <f>DATE(A2,B2,C2)</f>
         <v>1828</v>
       </c>
-      <c r="E2" s="4">
+      <c r="E2" s="1">
         <f t="shared" ref="E2:E8" si="0">D2</f>
         <v>1828</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F2" t="str">
+        <f ca="1">_xlfn.FORMULATEXT(D2)</f>
+        <v>=DATE(A2,B2,C2)</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2000</v>
       </c>
@@ -501,15 +509,19 @@
         <v>15</v>
       </c>
       <c r="D3" s="3">
-        <f t="shared" ref="D2:D8" si="1">DATE(A3,B3,C3)</f>
+        <f t="shared" ref="D3:D8" si="1">DATE(A3,B3,C3)</f>
         <v>36692</v>
       </c>
-      <c r="E3" s="4">
+      <c r="E3" s="1">
         <f t="shared" si="0"/>
         <v>36692</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F3" t="str">
+        <f t="shared" ref="F3:F9" ca="1" si="2">_xlfn.FORMULATEXT(D3)</f>
+        <v>=DATE(A3,B3,C3)</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2024</v>
       </c>
@@ -523,12 +535,16 @@
         <f t="shared" si="1"/>
         <v>45651</v>
       </c>
-      <c r="E4" s="4">
+      <c r="E4" s="1">
         <f t="shared" si="0"/>
         <v>45651</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F4" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>=DATE(A4,B4,C4)</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2025</v>
       </c>
@@ -542,12 +558,16 @@
         <f t="shared" si="1"/>
         <v>46016</v>
       </c>
-      <c r="E5" s="4">
+      <c r="E5" s="1">
         <f t="shared" si="0"/>
         <v>46016</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F5" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>=DATE(A5,B5,C5)</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2025.9</v>
       </c>
@@ -561,12 +581,16 @@
         <f t="shared" si="1"/>
         <v>46016</v>
       </c>
-      <c r="E6" s="4">
+      <c r="E6" s="1">
         <f t="shared" si="0"/>
         <v>46016</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F6" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>=DATE(A6,B6,C6)</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>2030</v>
       </c>
@@ -580,12 +604,16 @@
         <f t="shared" si="1"/>
         <v>47484</v>
       </c>
-      <c r="E7" s="4">
+      <c r="E7" s="1">
         <f t="shared" si="0"/>
         <v>47484</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F7" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>=DATE(A7,B7,C7)</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>9999</v>
       </c>
@@ -599,19 +627,27 @@
         <f t="shared" si="1"/>
         <v>2958465</v>
       </c>
-      <c r="E8" s="4">
+      <c r="E8" s="1">
         <f t="shared" si="0"/>
         <v>2958465</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F8" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>=DATE(A8,B8,C8)</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D9" s="3">
-        <f>DATE(2024, 11, 22)</f>
+        <f>DATE(2024,11,22)</f>
         <v>45618</v>
       </c>
-      <c r="E9" s="4">
+      <c r="E9" s="1">
         <f>D9</f>
         <v>45618</v>
+      </c>
+      <c r="F9" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>=DATE(2024,11,22)</v>
       </c>
     </row>
   </sheetData>

</xml_diff>